<commit_message>
Rework travel days calc method in cost module together with adding necessary methods in other modules. Still need some testing.
</commit_message>
<xml_diff>
--- a/test_data/railway_parameters.xlsx
+++ b/test_data/railway_parameters.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,14 @@
     <sheet name="categories" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">mobility!$A$1:$C$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">mobility!$A$1:$C$23</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="138">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Minimum distance an origin-destination pair cover to be derivable to railway (ton).</t>
   </si>
   <si>
-    <t>wagon_eac</t>
-  </si>
-  <si>
-    <t>locomotive_eac</t>
-  </si>
-  <si>
     <t>fuel_cost_by_km</t>
   </si>
   <si>
@@ -113,12 +107,6 @@
     <t>Fuel cost of running a locomotive one km (USD/km).</t>
   </si>
   <si>
-    <t>Equivalent anual cost of a locomotive. It must be calculated outside the model, from a spreadsheet (USD).</t>
-  </si>
-  <si>
-    <t>Equivalent anual cost of a wagon. It must be calculated outside the model, from a spreadsheet (USD).</t>
-  </si>
-  <si>
     <t>maintenance_by_locomotive</t>
   </si>
   <si>
@@ -131,12 +119,6 @@
     <t>Annual cost of a wagon maintenance (USD).</t>
   </si>
   <si>
-    <t>manpower_cost_by_loc_hour</t>
-  </si>
-  <si>
-    <t>Cost of conduction and guards manpower, by hour of locomotive running or waiting in turnout (USD/loc-hr).</t>
-  </si>
-  <si>
     <t>locom_head_stops_time</t>
   </si>
   <si>
@@ -149,9 +131,6 @@
     <t>max_derivation</t>
   </si>
   <si>
-    <t>Distance since probability of truck to rail derivation is maximum (km).</t>
-  </si>
-  <si>
     <t>dist_of_max_derivation</t>
   </si>
   <si>
@@ -164,9 +143,6 @@
     <t>tons_of_max_derivation</t>
   </si>
   <si>
-    <t>Tons since probability of truck to rail derivation is maximum (tons).</t>
-  </si>
-  <si>
     <t>coef_a_track_maint_cost</t>
   </si>
   <si>
@@ -407,12 +383,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>min_tons_to_be_derived</t>
-  </si>
-  <si>
-    <t>Minimum tons a road origin-destination pair must carry to be derivable to railway (ton).</t>
-  </si>
-  <si>
     <t>min_derivation</t>
   </si>
   <si>
@@ -422,18 +392,62 @@
     <t>Proportion of truck to rail derivation on the minimum distances and ton scale, ie minimum proportion of derivation (%).</t>
   </si>
   <si>
-    <t>Minimum tons that can be effectively derived in an origin-destination pair. If derivation calculation throws less than this threshold, od pair is not derivable (ton).</t>
+    <t>Minimum tons that must be derivable from a road origin-destination pair to be considered a derivable od pair (ton).</t>
+  </si>
+  <si>
+    <t>Distance since proportion of truck to rail derivation is maximum (km).</t>
+  </si>
+  <si>
+    <t>Road od tons since proportion of truck to rail derivation is maximum (tons).</t>
+  </si>
+  <si>
+    <t>manpower_cost_by_hour</t>
+  </si>
+  <si>
+    <t>manpower_by_loc</t>
+  </si>
+  <si>
+    <t>Cost of conduction and guards manpower, by hour (USD/hr).</t>
+  </si>
+  <si>
+    <t>Number of manpower needed to operate a single train (number).</t>
+  </si>
+  <si>
+    <t>locomotive_price</t>
+  </si>
+  <si>
+    <t>wagon_price</t>
+  </si>
+  <si>
+    <t>useful_life_wagon</t>
+  </si>
+  <si>
+    <t>useful_life_locom</t>
+  </si>
+  <si>
+    <t>Price of wagon (USD).</t>
+  </si>
+  <si>
+    <t>Price of a locomotive (USD).</t>
+  </si>
+  <si>
+    <t>Useful life a wagon (years).</t>
+  </si>
+  <si>
+    <t>Useful life a locomotive (years).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +470,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -474,10 +495,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -499,7 +521,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,9 +530,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -814,22 +839,22 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="97.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="97.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
@@ -838,7 +863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -849,7 +874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -860,9 +885,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>15</v>
@@ -871,18 +896,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -890,10 +915,10 @@
         <v>33.6</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -901,10 +926,10 @@
         <v>1276.8000000000002</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -915,7 +940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -926,7 +951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -934,7 +959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -945,7 +970,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -956,158 +981,191 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="5">
+        <v>80000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="5">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="5">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5">
-        <v>6463.835901091652</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="9">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="5">
+        <v>100170</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2487.6562500000005</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="5">
-        <v>154445.87620922364</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="7">
+        <v>15.21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="5">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="9">
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5">
-        <v>100170</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="5">
-        <v>2487.6562500000005</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="7">
-        <v>30.416666666666668</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="B23" s="4">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="4">
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="4">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="4">
         <v>100</v>
       </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="4">
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="4">
         <v>1.67</v>
       </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="5">
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="5">
         <v>420000</v>
       </c>
-      <c r="C24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="13">
+        <v>0.82</v>
+      </c>
+      <c r="C29" t="s">
         <v>111</v>
-      </c>
-      <c r="B25" s="4">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="13">
-        <v>0.82</v>
-      </c>
-      <c r="C26" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1124,10 +1182,10 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -1147,123 +1205,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4">
         <v>-0.62124999999999997</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4">
         <v>10.34046</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4">
         <v>-0.93081999999999998</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4">
         <v>458.46100000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4">
         <v>175000</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B7" s="4">
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B8" s="4">
         <v>0.08</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4">
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B10" s="5">
         <v>109500</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B11" s="5">
         <v>200000000</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5">
         <v>800000</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1274,51 +1332,51 @@
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B14" s="5">
         <v>1200000</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B15" s="10">
         <v>0.82</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B16" s="12">
         <v>156250.76923076919</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B17" s="12">
         <v>701400</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1334,14 +1392,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1357,68 +1415,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>0.11853075454128587</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B3">
         <v>0.5</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B4">
         <v>1.1752104423052856</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>1.5</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1431,16 +1489,16 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="83.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="83.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1458,11 +1516,11 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4">
-        <v>5000</v>
+      <c r="B2" s="5">
+        <v>7000</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1478,69 +1536,73 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B4" s="8">
         <v>0.8</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B5" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4">
         <v>500</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5">
         <v>120000</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" s="4">
-        <v>15000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
-      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1558,11 +1620,11 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="107.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="107.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1578,117 +1640,117 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B2" s="14">
         <v>0.8</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B3" s="14">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B4" s="14">
         <v>0.7</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B5" s="14">
         <v>0.6</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B6" s="14">
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>